<commit_message>
Removing DFC, FFC (easier to just command the angles & a collect)
</commit_message>
<xml_diff>
--- a/Command Dictionary.xlsx
+++ b/Command Dictionary.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HARP\Pointing-Camera\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlosj\Documents\HARP\Pointing-Camera\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E43549-32D2-4D5D-AD02-534E984D0EA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="14775"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
@@ -532,8 +531,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +541,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier Std"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Courier Std"/>
@@ -568,9 +582,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,11 +911,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,16 +1131,17 @@
       <c r="B11" t="s">
         <v>135</v>
       </c>
-      <c r="C11" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C11" s="2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1133,16 +1150,17 @@
       <c r="B12" t="s">
         <v>135</v>
       </c>
-      <c r="C12" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" s="2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -3777,7 +3795,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C256" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C256">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3787,7 +3805,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>